<commit_message>
BP MJP, Consolidated BSP IATA
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Performer_Email_S3\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 4\Traveloka_DataAutomation_Performer_Email_S4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150050E6-D237-4617-824B-34FC6829CAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69C900A-F26A-4100-BDD7-B4DD7DA8F668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>PathSaKey</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>SheetIdConfigChubb</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
   </si>
 </sst>
 </file>
@@ -2877,7 +2889,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2980,8 +2992,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>